<commit_message>
Binary Trees Easy Level Questions Completed
</commit_message>
<xml_diff>
--- a/DSA by Shradha Didi & Aman Bhaiya.xlsx
+++ b/DSA by Shradha Didi & Aman Bhaiya.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayes\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayes\Desktop\DSA-by-Shradha-Didi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46063C0-5E0A-43CB-BC46-80A371EAD9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56641B2-E1DE-4ADA-9FC2-FF7383D147FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,8 +22,8 @@
   </definedNames>
   <calcPr calcId="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{68AEC4D6-5B1A-4772-8735-C18A5469BEFD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{80F93246-4D64-4763-8AAB-1304371DD6DF}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{68AEC4D6-5B1A-4772-8735-C18A5469BEFD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -2519,8 +2519,8 @@
   </sheetPr>
   <dimension ref="A1:Z923"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A217" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D220" sqref="D220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="19.8" customHeight="1"/>
@@ -29452,13 +29452,13 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{80F93246-4D64-4763-8AAB-1304371DD6DF}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A293:C332" xr:uid="{677FEEB0-2285-45FE-90AA-2E1C977F17E8}"/>
+    </customSheetView>
     <customSheetView guid="{68AEC4D6-5B1A-4772-8735-C18A5469BEFD}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{7CA816E1-AA0A-4070-8E6E-FB79C1339065}"/>
-    </customSheetView>
-    <customSheetView guid="{80F93246-4D64-4763-8AAB-1304371DD6DF}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{4270B6FD-08DA-40A5-AF7F-A60912BC1C36}"/>
+      <autoFilter ref="A11:C37" xr:uid="{B290B4B3-3CCC-4BBC-B0BB-7AACE10C4F96}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="3">
@@ -30114,7 +30114,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17.399999999999999">
+    <row r="41" spans="1:2" ht="15.6">
       <c r="A41" s="3" t="s">
         <v>178</v>
       </c>
@@ -30122,7 +30122,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="17.399999999999999">
+    <row r="42" spans="1:2" ht="15.6">
       <c r="A42" s="3" t="s">
         <v>178</v>
       </c>
@@ -30130,11 +30130,11 @@
         <v>422</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17.399999999999999">
+    <row r="44" spans="1:2" ht="15.6">
       <c r="A44" s="16"/>
       <c r="B44" s="8"/>
     </row>
-    <row r="45" spans="1:2" ht="17.399999999999999">
+    <row r="45" spans="1:2" ht="15.6">
       <c r="A45" s="5" t="s">
         <v>201</v>
       </c>
@@ -30142,7 +30142,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="17.399999999999999">
+    <row r="46" spans="1:2" ht="15.6">
       <c r="A46" s="6" t="s">
         <v>201</v>
       </c>
@@ -30150,15 +30150,15 @@
         <v>424</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="17.399999999999999">
+    <row r="47" spans="1:2" ht="15.6">
       <c r="A47" s="16"/>
       <c r="B47" s="8"/>
     </row>
-    <row r="48" spans="1:2" ht="17.399999999999999">
+    <row r="48" spans="1:2" ht="15.6">
       <c r="A48" s="16"/>
       <c r="B48" s="8"/>
     </row>
-    <row r="49" spans="1:2" ht="17.399999999999999">
+    <row r="49" spans="1:2" ht="15.6">
       <c r="A49" s="3" t="s">
         <v>234</v>
       </c>
@@ -30166,7 +30166,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="17.399999999999999">
+    <row r="50" spans="1:2" ht="15.6">
       <c r="A50" s="16"/>
       <c r="B50" s="8"/>
     </row>

</xml_diff>